<commit_message>
implement create new sheet, fill staff id, deafult filepath
</commit_message>
<xml_diff>
--- a/ryan/salary/Feb-2016/salary-feb-2016.xlsx
+++ b/ryan/salary/Feb-2016/salary-feb-2016.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giang\Desktop\giang\salary\Feb-2016\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="HR" sheetId="1" r:id="rId1"/>
     <sheet name="Accounting" sheetId="2" r:id="rId2"/>
     <sheet name="QA" sheetId="3" r:id="rId3"/>
+    <sheet name="Manager" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>Staff ID</t>
   </si>
@@ -38,8 +34,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -67,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,7 +346,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -349,10 +354,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,6 +374,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -375,10 +391,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,6 +411,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -401,10 +423,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,6 +443,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>